<commit_message>
Updated "number_decimal" to "numbers_decimal"
</commit_message>
<xml_diff>
--- a/extras/test-form/plugin_test_form_text.xlsx
+++ b/extras/test-form/plugin_test_form_text.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max.s.haberman/Documents/Code/Other field plug-in repos/baseline-text/extras/test-form/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max.s.haberman/Documents/SurveyCTO code/Other field plug-in repos/baseline-text/extras/test-form/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7222E68C-D5F5-4245-844C-58777107FB76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5EF94FC-7B37-9D4C-B976-3EC80D4022F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="460" windowWidth="28800" windowHeight="16740" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="220" yWindow="500" windowWidth="28800" windowHeight="16620" tabRatio="534" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -2690,9 +2690,6 @@
     <t>This field has the &lt;i&gt;numbers_decimal&lt;/i&gt; appearance.</t>
   </si>
   <si>
-    <t>number_decimal</t>
-  </si>
-  <si>
     <t>appearance_phone</t>
   </si>
   <si>
@@ -2766,9 +2763,6 @@
   </si>
   <si>
     <t>numbers custom-baseline-text</t>
-  </si>
-  <si>
-    <t>number_decimal custom-baseline-text</t>
   </si>
   <si>
     <t>numbers_phone custom-baseline-text</t>
@@ -2853,6 +2847,12 @@
   </si>
   <si>
     <t>هذا له قيمة افتراضية وتلميح.</t>
+  </si>
+  <si>
+    <t>numbers_decimal</t>
+  </si>
+  <si>
+    <t>numbers_decimal custom-baseline-text</t>
   </si>
 </sst>
 </file>
@@ -3417,6 +3417,12 @@
     <xf numFmtId="0" fontId="16" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3449,12 +3455,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="108">
@@ -17508,9 +17508,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17791,16 +17791,16 @@
         <v>379</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>429</v>
-      </c>
-      <c r="D12" s="64" t="s">
-        <v>440</v>
+        <v>427</v>
+      </c>
+      <c r="D12" s="53" t="s">
+        <v>438</v>
       </c>
       <c r="E12" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="F12" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="13" spans="1:27" ht="34" x14ac:dyDescent="0.2">
@@ -17808,22 +17808,22 @@
         <v>87</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>429</v>
-      </c>
-      <c r="D13" s="64" t="s">
-        <v>440</v>
+        <v>427</v>
+      </c>
+      <c r="D13" s="53" t="s">
+        <v>438</v>
       </c>
       <c r="E13" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="F13" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="85" x14ac:dyDescent="0.2">
@@ -17836,14 +17836,14 @@
       <c r="C14" s="10" t="s">
         <v>381</v>
       </c>
-      <c r="D14" s="64" t="s">
-        <v>441</v>
+      <c r="D14" s="53" t="s">
+        <v>439</v>
       </c>
       <c r="E14" t="s">
         <v>382</v>
       </c>
       <c r="F14" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="85" x14ac:dyDescent="0.2">
@@ -17851,22 +17851,22 @@
         <v>87</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C15" s="10" t="s">
         <v>381</v>
       </c>
-      <c r="D15" s="64" t="s">
-        <v>441</v>
+      <c r="D15" s="53" t="s">
+        <v>439</v>
       </c>
       <c r="E15" t="s">
         <v>382</v>
       </c>
       <c r="F15" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="16" spans="1:27" ht="17" x14ac:dyDescent="0.2">
@@ -17880,16 +17880,16 @@
         <v>384</v>
       </c>
       <c r="D16" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E16" t="s">
         <v>382</v>
       </c>
-      <c r="F16" s="65" t="s">
-        <v>408</v>
+      <c r="F16" s="54" t="s">
+        <v>407</v>
       </c>
       <c r="G16" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="17" spans="1:22" ht="17" x14ac:dyDescent="0.2">
@@ -17897,25 +17897,25 @@
         <v>87</v>
       </c>
       <c r="B17" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C17" t="s">
         <v>384</v>
       </c>
       <c r="D17" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E17" t="s">
         <v>382</v>
       </c>
-      <c r="F17" s="65" t="s">
-        <v>408</v>
+      <c r="F17" s="54" t="s">
+        <v>407</v>
       </c>
       <c r="G17" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="18" spans="1:22" ht="51" x14ac:dyDescent="0.2">
@@ -17926,16 +17926,16 @@
         <v>385</v>
       </c>
       <c r="C18" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D18" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="I18" t="s">
         <v>386</v>
@@ -17946,22 +17946,22 @@
         <v>87</v>
       </c>
       <c r="B19" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C19" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D19" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="I19" t="s">
         <v>386</v>
@@ -17975,10 +17975,10 @@
         <v>367</v>
       </c>
       <c r="C20" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D20" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="N20" t="s">
         <v>387</v>
@@ -17989,16 +17989,16 @@
         <v>87</v>
       </c>
       <c r="B21" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C21" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="D21" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="N21" t="s">
         <v>387</v>
@@ -18009,13 +18009,13 @@
         <v>87</v>
       </c>
       <c r="B22" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C22" t="s">
         <v>390</v>
       </c>
       <c r="D22" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="Q22" t="s">
         <v>387</v>
@@ -18026,16 +18026,16 @@
         <v>87</v>
       </c>
       <c r="B23" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="C23" t="s">
         <v>390</v>
       </c>
       <c r="D23" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="Q23" t="s">
         <v>387</v>
@@ -18049,13 +18049,13 @@
         <v>389</v>
       </c>
       <c r="C24" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D24" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="Q24" t="s">
         <v>387</v>
@@ -18066,19 +18066,19 @@
         <v>87</v>
       </c>
       <c r="B25" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C25" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D25" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="Q25" t="s">
         <v>387</v>
@@ -18095,7 +18095,7 @@
         <v>391</v>
       </c>
       <c r="D26" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="T26" t="s">
         <v>392</v>
@@ -18106,16 +18106,16 @@
         <v>87</v>
       </c>
       <c r="B27" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C27" t="s">
         <v>391</v>
       </c>
       <c r="D27" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="T27" t="s">
         <v>392</v>
@@ -18132,7 +18132,7 @@
         <v>393</v>
       </c>
       <c r="D28" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="U28" t="s">
         <v>394</v>
@@ -18143,16 +18143,16 @@
         <v>87</v>
       </c>
       <c r="B29" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C29" t="s">
         <v>393</v>
       </c>
       <c r="D29" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="U29" t="s">
         <v>394</v>
@@ -18169,7 +18169,7 @@
         <v>395</v>
       </c>
       <c r="D30" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="V30" t="s">
         <v>396</v>
@@ -18180,16 +18180,16 @@
         <v>87</v>
       </c>
       <c r="B31" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C31" t="s">
         <v>395</v>
       </c>
       <c r="D31" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="H31" s="9" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="V31" t="s">
         <v>396</v>
@@ -18206,7 +18206,7 @@
         <v>398</v>
       </c>
       <c r="D32" s="21" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="H32" t="s">
         <v>88</v>
@@ -18217,16 +18217,16 @@
         <v>87</v>
       </c>
       <c r="B33" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C33" t="s">
         <v>398</v>
       </c>
       <c r="D33" s="21" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="H33" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="51" x14ac:dyDescent="0.2">
@@ -18240,10 +18240,10 @@
         <v>400</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="H34" t="s">
-        <v>401</v>
+        <v>452</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="51" x14ac:dyDescent="0.2">
@@ -18251,16 +18251,16 @@
         <v>87</v>
       </c>
       <c r="B35" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C35" t="s">
         <v>400</v>
       </c>
       <c r="D35" s="21" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="H35" t="s">
-        <v>427</v>
+        <v>453</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="51" x14ac:dyDescent="0.2">
@@ -18268,16 +18268,16 @@
         <v>87</v>
       </c>
       <c r="B36" t="s">
+        <v>401</v>
+      </c>
+      <c r="C36" t="s">
         <v>402</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" s="10" t="s">
+        <v>449</v>
+      </c>
+      <c r="H36" t="s">
         <v>403</v>
-      </c>
-      <c r="D36" s="10" t="s">
-        <v>451</v>
-      </c>
-      <c r="H36" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="51" x14ac:dyDescent="0.2">
@@ -18285,16 +18285,16 @@
         <v>87</v>
       </c>
       <c r="B37" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C37" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="H37" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="34" x14ac:dyDescent="0.2">
@@ -18302,28 +18302,28 @@
         <v>87</v>
       </c>
       <c r="B38" t="s">
+        <v>404</v>
+      </c>
+      <c r="C38" t="s">
         <v>405</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" s="10" t="s">
         <v>406</v>
-      </c>
-      <c r="D38" s="10" t="s">
-        <v>407</v>
       </c>
       <c r="E38" t="s">
         <v>382</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="I38" t="s">
         <v>386</v>
       </c>
       <c r="J38" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="K38" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="N38" t="s">
         <v>387</v>
@@ -18332,7 +18332,7 @@
         <v>388</v>
       </c>
       <c r="P38" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="34" x14ac:dyDescent="0.2">
@@ -18340,31 +18340,31 @@
         <v>87</v>
       </c>
       <c r="B39" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C39" t="s">
+        <v>405</v>
+      </c>
+      <c r="D39" s="10" t="s">
         <v>406</v>
-      </c>
-      <c r="D39" s="10" t="s">
-        <v>407</v>
       </c>
       <c r="E39" t="s">
         <v>382</v>
       </c>
       <c r="F39" s="11" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="H39" s="9" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="I39" t="s">
         <v>386</v>
       </c>
       <c r="J39" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="K39" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="N39" t="s">
         <v>387</v>
@@ -18373,7 +18373,7 @@
         <v>388</v>
       </c>
       <c r="P39" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
   </sheetData>
@@ -24739,14 +24739,14 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
+        <v>422</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>423</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>424</v>
       </c>
       <c r="C2" s="17" t="str">
         <f ca="1">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2005011406</v>
+        <v>2106112058</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>358</v>
@@ -24781,22 +24781,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="54"/>
+      <c r="B1" s="56"/>
       <c r="C1" s="32"/>
     </row>
     <row r="2" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="55"/>
-      <c r="B2" s="56"/>
+      <c r="A2" s="57"/>
+      <c r="B2" s="58"/>
       <c r="C2" s="32"/>
     </row>
     <row r="3" spans="1:30" s="33" customFormat="1" ht="97" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="58"/>
+      <c r="B3" s="60"/>
       <c r="C3" s="32"/>
     </row>
     <row r="4" spans="1:30" s="33" customFormat="1" x14ac:dyDescent="0.2">
@@ -24990,10 +24990,10 @@
       <c r="C7" s="32"/>
     </row>
     <row r="8" spans="1:30" s="42" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="61" t="s">
         <v>267</v>
       </c>
-      <c r="B8" s="59"/>
+      <c r="B8" s="61"/>
       <c r="C8" s="40"/>
       <c r="D8" s="41"/>
       <c r="E8" s="41"/>
@@ -27783,10 +27783,10 @@
       <c r="AD81" s="43"/>
     </row>
     <row r="83" spans="1:30" s="31" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="60" t="s">
+      <c r="A83" s="62" t="s">
         <v>263</v>
       </c>
-      <c r="B83" s="61"/>
+      <c r="B83" s="63"/>
       <c r="C83" s="26"/>
       <c r="D83" s="25"/>
       <c r="E83" s="30"/>
@@ -28946,20 +28946,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="33" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="55" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="54"/>
+      <c r="B1" s="56"/>
     </row>
     <row r="2" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="55"/>
-      <c r="B2" s="56"/>
+      <c r="A2" s="57"/>
+      <c r="B2" s="58"/>
     </row>
     <row r="3" spans="1:8" s="33" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="58"/>
+      <c r="B3" s="60"/>
     </row>
     <row r="4" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="5" spans="1:8" s="37" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -29034,28 +29034,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="64" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="63"/>
+      <c r="B1" s="65"/>
       <c r="C1" s="49"/>
       <c r="D1" s="49"/>
       <c r="E1" s="49"/>
       <c r="F1" s="49"/>
     </row>
     <row r="2" spans="1:8" s="33" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="55"/>
-      <c r="B2" s="56"/>
+      <c r="A2" s="57"/>
+      <c r="B2" s="58"/>
       <c r="C2" s="49"/>
       <c r="D2" s="49"/>
       <c r="E2" s="49"/>
       <c r="F2" s="49"/>
     </row>
     <row r="3" spans="1:8" s="33" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="58"/>
+      <c r="B3" s="60"/>
       <c r="C3" s="49"/>
       <c r="D3" s="49"/>
       <c r="E3" s="49"/>

</xml_diff>